<commit_message>
added deimuada.json, completed excel calendar
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,108 +424,1220 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Januar</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Februar</t>
+          <t>Oktober 25</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>März</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>April</t>
+          <t>November 25</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Mai</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Juni</t>
+          <t>Dezember 25</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Juli</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>August</t>
+          <t>Januar 26</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Oktober</t>
+          <t>Februar 26</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>März 26</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
-          <t>Dezember</t>
+          <t>April 26</t>
         </is>
       </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Mai 26</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Juni 26</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Juli 26</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>August 26</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>September 26</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="W4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" t="n">
+        <v>4</v>
+      </c>
+      <c r="U5" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5</v>
+      </c>
+      <c r="U6" t="n">
+        <v>5</v>
+      </c>
+      <c r="W6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6</v>
+      </c>
+      <c r="M7" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>6</v>
+      </c>
+      <c r="S7" t="n">
+        <v>6</v>
+      </c>
+      <c r="U7" t="n">
+        <v>6</v>
+      </c>
+      <c r="W7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" t="n">
+        <v>7</v>
+      </c>
+      <c r="M8" t="n">
+        <v>7</v>
+      </c>
+      <c r="O8" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>7</v>
+      </c>
+      <c r="S8" t="n">
+        <v>7</v>
+      </c>
+      <c r="U8" t="n">
+        <v>7</v>
+      </c>
+      <c r="W8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>8</v>
+      </c>
+      <c r="M9" t="n">
+        <v>8</v>
+      </c>
+      <c r="O9" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" t="n">
+        <v>8</v>
+      </c>
+      <c r="U9" t="n">
+        <v>8</v>
+      </c>
+      <c r="W9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9</v>
+      </c>
+      <c r="M10" t="n">
+        <v>9</v>
+      </c>
+      <c r="O10" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>9</v>
+      </c>
+      <c r="S10" t="n">
+        <v>9</v>
+      </c>
+      <c r="U10" t="n">
+        <v>9</v>
+      </c>
+      <c r="W10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" t="n">
+        <v>10</v>
+      </c>
+      <c r="K11" t="n">
+        <v>10</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10</v>
+      </c>
+      <c r="O11" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>10</v>
+      </c>
+      <c r="S11" t="n">
+        <v>10</v>
+      </c>
+      <c r="U11" t="n">
+        <v>10</v>
+      </c>
+      <c r="W11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G12" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" t="n">
+        <v>11</v>
+      </c>
+      <c r="K12" t="n">
+        <v>11</v>
+      </c>
+      <c r="M12" t="n">
+        <v>11</v>
+      </c>
+      <c r="O12" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>11</v>
+      </c>
+      <c r="S12" t="n">
+        <v>11</v>
+      </c>
+      <c r="U12" t="n">
+        <v>11</v>
+      </c>
+      <c r="W12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" t="n">
+        <v>12</v>
+      </c>
+      <c r="K13" t="n">
+        <v>12</v>
+      </c>
+      <c r="M13" t="n">
+        <v>12</v>
+      </c>
+      <c r="O13" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>12</v>
+      </c>
+      <c r="S13" t="n">
+        <v>12</v>
+      </c>
+      <c r="U13" t="n">
+        <v>12</v>
+      </c>
+      <c r="W13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13</v>
+      </c>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
+      <c r="G14" t="n">
+        <v>13</v>
+      </c>
+      <c r="I14" t="n">
+        <v>13</v>
+      </c>
+      <c r="K14" t="n">
+        <v>13</v>
+      </c>
+      <c r="M14" t="n">
+        <v>13</v>
+      </c>
+      <c r="O14" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>13</v>
+      </c>
+      <c r="S14" t="n">
+        <v>13</v>
+      </c>
+      <c r="U14" t="n">
+        <v>13</v>
+      </c>
+      <c r="W14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G15" t="n">
+        <v>14</v>
+      </c>
+      <c r="I15" t="n">
+        <v>14</v>
+      </c>
+      <c r="K15" t="n">
+        <v>14</v>
+      </c>
+      <c r="M15" t="n">
+        <v>14</v>
+      </c>
+      <c r="O15" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>14</v>
+      </c>
+      <c r="S15" t="n">
+        <v>14</v>
+      </c>
+      <c r="U15" t="n">
+        <v>14</v>
+      </c>
+      <c r="W15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="I16" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" t="n">
+        <v>15</v>
+      </c>
+      <c r="M16" t="n">
+        <v>15</v>
+      </c>
+      <c r="O16" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>15</v>
+      </c>
+      <c r="S16" t="n">
+        <v>15</v>
+      </c>
+      <c r="U16" t="n">
+        <v>15</v>
+      </c>
+      <c r="W16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16</v>
+      </c>
+      <c r="I17" t="n">
+        <v>16</v>
+      </c>
+      <c r="K17" t="n">
+        <v>16</v>
+      </c>
+      <c r="M17" t="n">
+        <v>16</v>
+      </c>
+      <c r="O17" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>16</v>
+      </c>
+      <c r="S17" t="n">
+        <v>16</v>
+      </c>
+      <c r="U17" t="n">
+        <v>16</v>
+      </c>
+      <c r="W17" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+      <c r="E18" t="n">
+        <v>17</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17</v>
+      </c>
+      <c r="I18" t="n">
+        <v>17</v>
+      </c>
+      <c r="K18" t="n">
+        <v>17</v>
+      </c>
+      <c r="M18" t="n">
+        <v>17</v>
+      </c>
+      <c r="O18" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>17</v>
+      </c>
+      <c r="S18" t="n">
+        <v>17</v>
+      </c>
+      <c r="U18" t="n">
+        <v>17</v>
+      </c>
+      <c r="W18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" t="n">
+        <v>18</v>
+      </c>
+      <c r="G19" t="n">
+        <v>18</v>
+      </c>
+      <c r="I19" t="n">
+        <v>18</v>
+      </c>
+      <c r="K19" t="n">
+        <v>18</v>
+      </c>
+      <c r="M19" t="n">
+        <v>18</v>
+      </c>
+      <c r="O19" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>18</v>
+      </c>
+      <c r="S19" t="n">
+        <v>18</v>
+      </c>
+      <c r="U19" t="n">
+        <v>18</v>
+      </c>
+      <c r="W19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>19</v>
+      </c>
+      <c r="E20" t="n">
+        <v>19</v>
+      </c>
+      <c r="G20" t="n">
+        <v>19</v>
+      </c>
+      <c r="I20" t="n">
+        <v>19</v>
+      </c>
+      <c r="K20" t="n">
+        <v>19</v>
+      </c>
+      <c r="M20" t="n">
+        <v>19</v>
+      </c>
+      <c r="O20" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>19</v>
+      </c>
+      <c r="S20" t="n">
+        <v>19</v>
+      </c>
+      <c r="U20" t="n">
+        <v>19</v>
+      </c>
+      <c r="W20" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" t="n">
+        <v>20</v>
+      </c>
+      <c r="K21" t="n">
+        <v>20</v>
+      </c>
+      <c r="M21" t="n">
+        <v>20</v>
+      </c>
+      <c r="O21" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>20</v>
+      </c>
+      <c r="S21" t="n">
+        <v>20</v>
+      </c>
+      <c r="U21" t="n">
+        <v>20</v>
+      </c>
+      <c r="W21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>21</v>
+      </c>
+      <c r="E22" t="n">
+        <v>21</v>
+      </c>
+      <c r="G22" t="n">
+        <v>21</v>
+      </c>
+      <c r="I22" t="n">
+        <v>21</v>
+      </c>
+      <c r="K22" t="n">
+        <v>21</v>
+      </c>
+      <c r="M22" t="n">
+        <v>21</v>
+      </c>
+      <c r="O22" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>21</v>
+      </c>
+      <c r="S22" t="n">
+        <v>21</v>
+      </c>
+      <c r="U22" t="n">
+        <v>21</v>
+      </c>
+      <c r="W22" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>22</v>
+      </c>
+      <c r="E23" t="n">
+        <v>22</v>
+      </c>
+      <c r="G23" t="n">
+        <v>22</v>
+      </c>
+      <c r="I23" t="n">
+        <v>22</v>
+      </c>
+      <c r="K23" t="n">
+        <v>22</v>
+      </c>
+      <c r="M23" t="n">
+        <v>22</v>
+      </c>
+      <c r="O23" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>22</v>
+      </c>
+      <c r="S23" t="n">
+        <v>22</v>
+      </c>
+      <c r="U23" t="n">
+        <v>22</v>
+      </c>
+      <c r="W23" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>23</v>
+      </c>
+      <c r="E24" t="n">
+        <v>23</v>
+      </c>
+      <c r="G24" t="n">
+        <v>23</v>
+      </c>
+      <c r="I24" t="n">
+        <v>23</v>
+      </c>
+      <c r="K24" t="n">
+        <v>23</v>
+      </c>
+      <c r="M24" t="n">
+        <v>23</v>
+      </c>
+      <c r="O24" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>23</v>
+      </c>
+      <c r="S24" t="n">
+        <v>23</v>
+      </c>
+      <c r="U24" t="n">
+        <v>23</v>
+      </c>
+      <c r="W24" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" t="n">
+        <v>24</v>
+      </c>
+      <c r="G25" t="n">
+        <v>24</v>
+      </c>
+      <c r="I25" t="n">
+        <v>24</v>
+      </c>
+      <c r="K25" t="n">
+        <v>24</v>
+      </c>
+      <c r="M25" t="n">
+        <v>24</v>
+      </c>
+      <c r="O25" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>24</v>
+      </c>
+      <c r="S25" t="n">
+        <v>24</v>
+      </c>
+      <c r="U25" t="n">
+        <v>24</v>
+      </c>
+      <c r="W25" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nwq sodif</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="C26" t="n">
+        <v>25</v>
+      </c>
+      <c r="E26" t="n">
+        <v>25</v>
+      </c>
+      <c r="G26" t="n">
+        <v>25</v>
+      </c>
+      <c r="I26" t="n">
+        <v>25</v>
+      </c>
+      <c r="K26" t="n">
+        <v>25</v>
+      </c>
+      <c r="M26" t="n">
+        <v>25</v>
+      </c>
+      <c r="O26" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>25</v>
+      </c>
+      <c r="S26" t="n">
+        <v>25</v>
+      </c>
+      <c r="U26" t="n">
+        <v>25</v>
+      </c>
+      <c r="W26" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>lsdkjfl</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Charlie</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>234</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>csdf</t>
-        </is>
+      <c r="C27" t="n">
+        <v>26</v>
+      </c>
+      <c r="E27" t="n">
+        <v>26</v>
+      </c>
+      <c r="G27" t="n">
+        <v>26</v>
+      </c>
+      <c r="I27" t="n">
+        <v>26</v>
+      </c>
+      <c r="K27" t="n">
+        <v>26</v>
+      </c>
+      <c r="M27" t="n">
+        <v>26</v>
+      </c>
+      <c r="O27" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>26</v>
+      </c>
+      <c r="S27" t="n">
+        <v>26</v>
+      </c>
+      <c r="U27" t="n">
+        <v>26</v>
+      </c>
+      <c r="W27" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>27</v>
+      </c>
+      <c r="E28" t="n">
+        <v>27</v>
+      </c>
+      <c r="G28" t="n">
+        <v>27</v>
+      </c>
+      <c r="I28" t="n">
+        <v>27</v>
+      </c>
+      <c r="K28" t="n">
+        <v>27</v>
+      </c>
+      <c r="M28" t="n">
+        <v>27</v>
+      </c>
+      <c r="O28" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>27</v>
+      </c>
+      <c r="S28" t="n">
+        <v>27</v>
+      </c>
+      <c r="U28" t="n">
+        <v>27</v>
+      </c>
+      <c r="W28" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>28</v>
+      </c>
+      <c r="E29" t="n">
+        <v>28</v>
+      </c>
+      <c r="G29" t="n">
+        <v>28</v>
+      </c>
+      <c r="I29" t="n">
+        <v>28</v>
+      </c>
+      <c r="K29" t="n">
+        <v>28</v>
+      </c>
+      <c r="M29" t="n">
+        <v>28</v>
+      </c>
+      <c r="O29" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>28</v>
+      </c>
+      <c r="S29" t="n">
+        <v>28</v>
+      </c>
+      <c r="U29" t="n">
+        <v>28</v>
+      </c>
+      <c r="W29" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>29</v>
+      </c>
+      <c r="E30" t="n">
+        <v>29</v>
+      </c>
+      <c r="G30" t="n">
+        <v>29</v>
+      </c>
+      <c r="K30" t="n">
+        <v>29</v>
+      </c>
+      <c r="M30" t="n">
+        <v>29</v>
+      </c>
+      <c r="O30" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>29</v>
+      </c>
+      <c r="S30" t="n">
+        <v>29</v>
+      </c>
+      <c r="U30" t="n">
+        <v>29</v>
+      </c>
+      <c r="W30" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>30</v>
+      </c>
+      <c r="E31" t="n">
+        <v>30</v>
+      </c>
+      <c r="G31" t="n">
+        <v>30</v>
+      </c>
+      <c r="K31" t="n">
+        <v>30</v>
+      </c>
+      <c r="M31" t="n">
+        <v>30</v>
+      </c>
+      <c r="O31" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>30</v>
+      </c>
+      <c r="S31" t="n">
+        <v>30</v>
+      </c>
+      <c r="U31" t="n">
+        <v>30</v>
+      </c>
+      <c r="W31" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="E32" t="n">
+        <v>31</v>
+      </c>
+      <c r="G32" t="n">
+        <v>31</v>
+      </c>
+      <c r="K32" t="n">
+        <v>31</v>
+      </c>
+      <c r="O32" t="n">
+        <v>31</v>
+      </c>
+      <c r="S32" t="n">
+        <v>31</v>
+      </c>
+      <c r="U32" t="n">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct data with adjusted with
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -413,13 +413,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="4" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="4" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="4" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="4" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="4" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="4" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="4" customWidth="1" min="15" max="15"/>
+    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="4" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="4" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="4" customWidth="1" min="21" max="21"/>
+    <col width="15" customWidth="1" min="22" max="22"/>
+    <col width="4" customWidth="1" min="23" max="23"/>
+    <col width="15" customWidth="1" min="24" max="24"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -543,6 +568,11 @@
       <c r="M3" t="n">
         <v>2</v>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="O3" t="n">
         <v>2</v>
       </c>
@@ -590,11 +620,21 @@
       <c r="S4" t="n">
         <v>3</v>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="U4" t="n">
         <v>3</v>
       </c>
       <c r="W4" t="n">
         <v>3</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -631,6 +671,11 @@
       <c r="U5" t="n">
         <v>4</v>
       </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="W5" t="n">
         <v>4</v>
       </c>
@@ -651,6 +696,11 @@
       <c r="I6" t="n">
         <v>5</v>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="K6" t="n">
         <v>5</v>
       </c>
@@ -663,8 +713,18 @@
       <c r="Q6" t="n">
         <v>5</v>
       </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="S6" t="n">
         <v>5</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="U6" t="n">
         <v>5</v>
@@ -686,6 +746,11 @@
       <c r="G7" t="n">
         <v>6</v>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>6</v>
       </c>
@@ -695,8 +760,18 @@
       <c r="M7" t="n">
         <v>6</v>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="O7" t="n">
         <v>6</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="Q7" t="n">
         <v>6</v>
@@ -718,9 +793,19 @@
       <c r="C8" t="n">
         <v>7</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="E8" t="n">
         <v>7</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="G8" t="n">
         <v>7</v>
       </c>
@@ -729,6 +814,11 @@
       </c>
       <c r="K8" t="n">
         <v>7</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="M8" t="n">
         <v>7</v>
@@ -759,6 +849,11 @@
       <c r="E9" t="n">
         <v>8</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="G9" t="n">
         <v>8</v>
       </c>
@@ -844,6 +939,11 @@
       <c r="K11" t="n">
         <v>10</v>
       </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="M11" t="n">
         <v>10</v>
       </c>
@@ -853,6 +953,11 @@
       <c r="Q11" t="n">
         <v>10</v>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="S11" t="n">
         <v>10</v>
       </c>
@@ -861,6 +966,11 @@
       </c>
       <c r="W11" t="n">
         <v>10</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1022,6 +1132,11 @@
       <c r="C16" t="n">
         <v>15</v>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="E16" t="n">
         <v>15</v>
       </c>
@@ -1030,6 +1145,11 @@
       </c>
       <c r="I16" t="n">
         <v>15</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
       </c>
       <c r="K16" t="n">
         <v>15</v>
@@ -1154,6 +1274,11 @@
       <c r="O19" t="n">
         <v>18</v>
       </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="Q19" t="n">
         <v>18</v>
       </c>
@@ -1163,8 +1288,18 @@
       <c r="U19" t="n">
         <v>18</v>
       </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="W19" t="n">
         <v>18</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1201,6 +1336,11 @@
       <c r="U20" t="n">
         <v>19</v>
       </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="W20" t="n">
         <v>19</v>
       </c>
@@ -1221,6 +1361,11 @@
       <c r="I21" t="n">
         <v>20</v>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="K21" t="n">
         <v>20</v>
       </c>
@@ -1233,8 +1378,18 @@
       <c r="Q21" t="n">
         <v>20</v>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="S21" t="n">
         <v>20</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="U21" t="n">
         <v>20</v>
@@ -1256,6 +1411,11 @@
       <c r="G22" t="n">
         <v>21</v>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="I22" t="n">
         <v>21</v>
       </c>
@@ -1265,8 +1425,18 @@
       <c r="M22" t="n">
         <v>21</v>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="O22" t="n">
         <v>21</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="Q22" t="n">
         <v>21</v>
@@ -1288,9 +1458,19 @@
       <c r="C23" t="n">
         <v>22</v>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="E23" t="n">
         <v>22</v>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
+      </c>
       <c r="G23" t="n">
         <v>22</v>
       </c>
@@ -1299,6 +1479,11 @@
       </c>
       <c r="K23" t="n">
         <v>22</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Gar | Kin | Sch</t>
+        </is>
       </c>
       <c r="M23" t="n">
         <v>22</v>
@@ -1332,6 +1517,11 @@
       <c r="G24" t="n">
         <v>23</v>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="I24" t="n">
         <v>23</v>
       </c>
@@ -1417,6 +1607,11 @@
       <c r="M26" t="n">
         <v>25</v>
       </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="O26" t="n">
         <v>25</v>
       </c>
@@ -1464,6 +1659,11 @@
       <c r="S27" t="n">
         <v>26</v>
       </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="U27" t="n">
         <v>26</v>
       </c>
@@ -1624,6 +1824,11 @@
       <c r="E32" t="n">
         <v>31</v>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Kue</t>
+        </is>
+      </c>
       <c r="G32" t="n">
         <v>31</v>
       </c>
@@ -1641,6 +1846,20 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved format for data input
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -423,27 +423,27 @@
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="4" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="4" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
     <col width="4" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
     <col width="4" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
     <col width="4" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
     <col width="4" customWidth="1" min="13" max="13"/>
-    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
     <col width="4" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="16" max="16"/>
     <col width="4" customWidth="1" min="17" max="17"/>
-    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
     <col width="4" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
     <col width="4" customWidth="1" min="21" max="21"/>
-    <col width="15" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
     <col width="4" customWidth="1" min="23" max="23"/>
-    <col width="15" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -518,14 +518,14 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Kue</t>
-        </is>
-      </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
@@ -535,20 +535,45 @@
       <c r="M2" t="n">
         <v>1</v>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="O2" t="n">
         <v>1</v>
       </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="Q2" t="n">
         <v>1</v>
       </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="S2" t="n">
         <v>1</v>
       </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="U2" t="n">
         <v>1</v>
       </c>
       <c r="W2" t="n">
         <v>1</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -561,15 +586,35 @@
       <c r="E3" t="n">
         <v>2</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="G3" t="n">
         <v>2</v>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="I3" t="n">
         <v>2</v>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="M3" t="n">
         <v>2</v>
       </c>
@@ -579,6 +624,11 @@
       <c r="Q3" t="n">
         <v>2</v>
       </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="S3" t="n">
         <v>2</v>
       </c>
@@ -587,6 +637,11 @@
       </c>
       <c r="W3" t="n">
         <v>2</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -596,24 +651,44 @@
       <c r="C4" t="n">
         <v>3</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="E4" t="n">
         <v>3</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="G4" t="n">
         <v>3</v>
       </c>
       <c r="I4" t="n">
         <v>3</v>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="K4" t="n">
         <v>3</v>
       </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="M4" t="n">
         <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Vor</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -622,11 +697,26 @@
       <c r="Q4" t="n">
         <v>3</v>
       </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="S4" t="n">
         <v>3</v>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="U4" t="n">
         <v>3</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
       <c r="W4" t="n">
         <v>3</v>
@@ -639,6 +729,11 @@
       <c r="C5" t="n">
         <v>4</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
@@ -648,35 +743,50 @@
       <c r="I5" t="n">
         <v>4</v>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="K5" t="n">
         <v>4</v>
       </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="M5" t="n">
         <v>4</v>
       </c>
       <c r="O5" t="n">
         <v>4</v>
       </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="Q5" t="n">
         <v>4</v>
       </c>
       <c r="S5" t="n">
         <v>4</v>
       </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Kue</t>
-        </is>
-      </c>
       <c r="U5" t="n">
         <v>4</v>
       </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="W5" t="n">
         <v>4</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Vor</t>
         </is>
       </c>
     </row>
@@ -687,12 +797,27 @@
       <c r="C6" t="n">
         <v>5</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="E6" t="n">
         <v>5</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="G6" t="n">
         <v>5</v>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="I6" t="n">
         <v>5</v>
       </c>
@@ -705,9 +830,19 @@
       <c r="O6" t="n">
         <v>5</v>
       </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="Q6" t="n">
         <v>5</v>
       </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="S6" t="n">
         <v>5</v>
       </c>
@@ -716,7 +851,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Sch</t>
         </is>
       </c>
       <c r="W6" t="n">
@@ -736,37 +871,52 @@
       <c r="G7" t="n">
         <v>6</v>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>6</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Vor</t>
         </is>
       </c>
       <c r="K7" t="n">
         <v>6</v>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="M7" t="n">
         <v>6</v>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="O7" t="n">
         <v>6</v>
       </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="Q7" t="n">
         <v>6</v>
       </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="S7" t="n">
         <v>6</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="U7" t="n">
@@ -783,6 +933,11 @@
       <c r="C8" t="n">
         <v>7</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="E8" t="n">
         <v>7</v>
       </c>
@@ -791,7 +946,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Sch</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -805,28 +960,38 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="O8" t="n">
         <v>7</v>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="Q8" t="n">
         <v>7</v>
       </c>
       <c r="S8" t="n">
         <v>7</v>
       </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="U8" t="n">
         <v>7</v>
       </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="W8" t="n">
         <v>7</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Bad | Kin</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -836,17 +1001,12 @@
       <c r="C9" t="n">
         <v>8</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="E9" t="n">
         <v>8</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -858,28 +1018,53 @@
       <c r="K9" t="n">
         <v>8</v>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="M9" t="n">
         <v>8</v>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="O9" t="n">
         <v>8</v>
       </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="Q9" t="n">
         <v>8</v>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="S9" t="n">
         <v>8</v>
       </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="U9" t="n">
         <v>8</v>
       </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="W9" t="n">
         <v>8</v>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -894,18 +1079,33 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="G10" t="n">
         <v>9</v>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="I10" t="n">
         <v>9</v>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Bad | Kin</t>
+        </is>
+      </c>
       <c r="K10" t="n">
         <v>9</v>
       </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="M10" t="n">
         <v>9</v>
       </c>
@@ -915,14 +1115,29 @@
       <c r="Q10" t="n">
         <v>9</v>
       </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Kin | WC</t>
+        </is>
+      </c>
       <c r="S10" t="n">
         <v>9</v>
       </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="U10" t="n">
         <v>9</v>
       </c>
       <c r="W10" t="n">
         <v>9</v>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -932,35 +1147,90 @@
       <c r="C11" t="n">
         <v>10</v>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="G11" t="n">
         <v>10</v>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="I11" t="n">
         <v>10</v>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="K11" t="n">
         <v>10</v>
       </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="M11" t="n">
         <v>10</v>
       </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Kin | Vor</t>
+        </is>
+      </c>
       <c r="O11" t="n">
         <v>10</v>
       </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="Q11" t="n">
         <v>10</v>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="S11" t="n">
         <v>10</v>
       </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="U11" t="n">
         <v>10</v>
       </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="W11" t="n">
         <v>10</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -970,21 +1240,36 @@
       <c r="C12" t="n">
         <v>11</v>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Kin | WC</t>
+        </is>
+      </c>
       <c r="E12" t="n">
         <v>11</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="G12" t="n">
         <v>11</v>
       </c>
       <c r="I12" t="n">
         <v>11</v>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="K12" t="n">
         <v>11</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Kin | Sch</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -993,26 +1278,31 @@
       <c r="O12" t="n">
         <v>11</v>
       </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="Q12" t="n">
         <v>11</v>
       </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Kue</t>
-        </is>
-      </c>
       <c r="S12" t="n">
         <v>11</v>
       </c>
       <c r="U12" t="n">
         <v>11</v>
       </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>WC | Woh</t>
+        </is>
+      </c>
       <c r="W12" t="n">
         <v>11</v>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Vor</t>
         </is>
       </c>
     </row>
@@ -1023,15 +1313,35 @@
       <c r="C13" t="n">
         <v>12</v>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="E13" t="n">
         <v>12</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="G13" t="n">
         <v>12</v>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="I13" t="n">
         <v>12</v>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="K13" t="n">
         <v>12</v>
       </c>
@@ -1041,14 +1351,34 @@
       <c r="O13" t="n">
         <v>12</v>
       </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="Q13" t="n">
         <v>12</v>
       </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Vor | Woh</t>
+        </is>
+      </c>
       <c r="S13" t="n">
         <v>12</v>
       </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="U13" t="n">
         <v>12</v>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
       </c>
       <c r="W13" t="n">
         <v>12</v>
@@ -1067,23 +1397,53 @@
       <c r="G14" t="n">
         <v>13</v>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>WC | Woh</t>
+        </is>
+      </c>
       <c r="I14" t="n">
         <v>13</v>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="K14" t="n">
         <v>13</v>
       </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="M14" t="n">
         <v>13</v>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Bad | Woh</t>
+        </is>
+      </c>
       <c r="O14" t="n">
         <v>13</v>
       </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Sch | Woh</t>
+        </is>
+      </c>
       <c r="Q14" t="n">
         <v>13</v>
       </c>
       <c r="S14" t="n">
         <v>13</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
       <c r="U14" t="n">
         <v>13</v>
@@ -1099,21 +1459,46 @@
       <c r="C15" t="n">
         <v>14</v>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Vor | Woh</t>
+        </is>
+      </c>
       <c r="E15" t="n">
         <v>14</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="G15" t="n">
         <v>14</v>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="I15" t="n">
         <v>14</v>
       </c>
       <c r="K15" t="n">
         <v>14</v>
       </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="M15" t="n">
         <v>14</v>
       </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="O15" t="n">
         <v>14</v>
       </c>
@@ -1123,11 +1508,26 @@
       <c r="S15" t="n">
         <v>14</v>
       </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="U15" t="n">
         <v>14</v>
       </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="W15" t="n">
         <v>14</v>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1140,6 +1540,11 @@
       <c r="E16" t="n">
         <v>15</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="G16" t="n">
         <v>15</v>
       </c>
@@ -1152,20 +1557,45 @@
       <c r="M16" t="n">
         <v>15</v>
       </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="O16" t="n">
         <v>15</v>
       </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="Q16" t="n">
         <v>15</v>
       </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="S16" t="n">
         <v>15</v>
       </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="U16" t="n">
         <v>15</v>
       </c>
       <c r="W16" t="n">
         <v>15</v>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1175,28 +1605,38 @@
       <c r="C17" t="n">
         <v>16</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Kue</t>
-        </is>
-      </c>
       <c r="E17" t="n">
         <v>16</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="G17" t="n">
         <v>16</v>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="I17" t="n">
         <v>16</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="K17" t="n">
         <v>16</v>
       </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="M17" t="n">
         <v>16</v>
       </c>
@@ -1206,6 +1646,11 @@
       <c r="Q17" t="n">
         <v>16</v>
       </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="S17" t="n">
         <v>16</v>
       </c>
@@ -1214,6 +1659,11 @@
       </c>
       <c r="W17" t="n">
         <v>16</v>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1223,32 +1673,72 @@
       <c r="C18" t="n">
         <v>17</v>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="E18" t="n">
         <v>17</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="G18" t="n">
         <v>17</v>
       </c>
       <c r="I18" t="n">
         <v>17</v>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="K18" t="n">
         <v>17</v>
       </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="M18" t="n">
         <v>17</v>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="O18" t="n">
         <v>17</v>
       </c>
       <c r="Q18" t="n">
         <v>17</v>
       </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="S18" t="n">
         <v>17</v>
       </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="U18" t="n">
         <v>17</v>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
       <c r="W18" t="n">
         <v>17</v>
@@ -1261,6 +1751,11 @@
       <c r="C19" t="n">
         <v>18</v>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="E19" t="n">
         <v>18</v>
       </c>
@@ -1270,15 +1765,30 @@
       <c r="I19" t="n">
         <v>18</v>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="K19" t="n">
         <v>18</v>
       </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="M19" t="n">
         <v>18</v>
       </c>
       <c r="O19" t="n">
         <v>18</v>
       </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="Q19" t="n">
         <v>18</v>
       </c>
@@ -1288,8 +1798,18 @@
       <c r="U19" t="n">
         <v>18</v>
       </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="W19" t="n">
         <v>18</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1299,12 +1819,27 @@
       <c r="C20" t="n">
         <v>19</v>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="E20" t="n">
         <v>19</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="G20" t="n">
         <v>19</v>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="I20" t="n">
         <v>19</v>
       </c>
@@ -1319,12 +1854,17 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="Q20" t="n">
         <v>19</v>
       </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="S20" t="n">
         <v>19</v>
       </c>
@@ -1333,16 +1873,11 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Sch</t>
         </is>
       </c>
       <c r="W20" t="n">
         <v>19</v>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
       </c>
     </row>
     <row r="21">
@@ -1358,31 +1893,56 @@
       <c r="G21" t="n">
         <v>20</v>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>20</v>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="K21" t="n">
         <v>20</v>
       </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="M21" t="n">
         <v>20</v>
       </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="O21" t="n">
         <v>20</v>
       </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="Q21" t="n">
         <v>20</v>
       </c>
       <c r="S21" t="n">
         <v>20</v>
       </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="U21" t="n">
         <v>20</v>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
       </c>
       <c r="W21" t="n">
         <v>20</v>
@@ -1395,50 +1955,65 @@
       <c r="C22" t="n">
         <v>21</v>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="E22" t="n">
         <v>21</v>
       </c>
       <c r="G22" t="n">
         <v>21</v>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="I22" t="n">
         <v>21</v>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="K22" t="n">
         <v>21</v>
       </c>
       <c r="M22" t="n">
         <v>21</v>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="O22" t="n">
         <v>21</v>
       </c>
       <c r="Q22" t="n">
         <v>21</v>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="S22" t="n">
         <v>21</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="U22" t="n">
         <v>21</v>
       </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="W22" t="n">
         <v>21</v>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1451,14 +2026,14 @@
       <c r="E23" t="n">
         <v>22</v>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="G23" t="n">
         <v>22</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="I23" t="n">
         <v>22</v>
       </c>
@@ -1470,7 +2045,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Sch</t>
         </is>
       </c>
       <c r="O23" t="n">
@@ -1478,20 +2053,35 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Vor</t>
         </is>
       </c>
       <c r="Q23" t="n">
         <v>22</v>
       </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="S23" t="n">
         <v>22</v>
       </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="U23" t="n">
         <v>22</v>
       </c>
       <c r="W23" t="n">
         <v>22</v>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Kin | WC</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1501,31 +2091,36 @@
       <c r="C24" t="n">
         <v>23</v>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Gar | Kin | Sch</t>
-        </is>
-      </c>
       <c r="E24" t="n">
         <v>23</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>WC</t>
         </is>
       </c>
       <c r="G24" t="n">
         <v>23</v>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="I24" t="n">
         <v>23</v>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="K24" t="n">
         <v>23</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Gar | Kin | Sch</t>
+          <t>Bad</t>
         </is>
       </c>
       <c r="M24" t="n">
@@ -1537,14 +2132,29 @@
       <c r="Q24" t="n">
         <v>23</v>
       </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="S24" t="n">
         <v>23</v>
       </c>
       <c r="U24" t="n">
         <v>23</v>
       </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="W24" t="n">
         <v>23</v>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>Sch | Tec</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1554,40 +2164,80 @@
       <c r="C25" t="n">
         <v>24</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="E25" t="n">
         <v>24</v>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="G25" t="n">
         <v>24</v>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Kue</t>
-        </is>
-      </c>
       <c r="I25" t="n">
         <v>24</v>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Kin | WC</t>
+        </is>
+      </c>
       <c r="K25" t="n">
         <v>24</v>
       </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="M25" t="n">
         <v>24</v>
       </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="O25" t="n">
         <v>24</v>
       </c>
       <c r="Q25" t="n">
         <v>24</v>
       </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Kin | Sch</t>
+        </is>
+      </c>
       <c r="S25" t="n">
         <v>24</v>
       </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Kin | Vor</t>
+        </is>
+      </c>
       <c r="U25" t="n">
         <v>24</v>
       </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Bad | Tec</t>
+        </is>
+      </c>
       <c r="W25" t="n">
         <v>24</v>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>Gar</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1597,35 +2247,85 @@
       <c r="C26" t="n">
         <v>25</v>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="E26" t="n">
         <v>25</v>
       </c>
       <c r="G26" t="n">
         <v>25</v>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="I26" t="n">
         <v>25</v>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Sch | Tec</t>
+        </is>
+      </c>
       <c r="K26" t="n">
         <v>25</v>
       </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="M26" t="n">
         <v>25</v>
       </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="O26" t="n">
         <v>25</v>
       </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Bad | Kin</t>
+        </is>
+      </c>
       <c r="Q26" t="n">
         <v>25</v>
       </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Tec</t>
+        </is>
+      </c>
       <c r="S26" t="n">
         <v>25</v>
       </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Tec</t>
+        </is>
+      </c>
       <c r="U26" t="n">
         <v>25</v>
       </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Gar | WC</t>
+        </is>
+      </c>
       <c r="W26" t="n">
         <v>25</v>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>Vor | Woh</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1635,40 +2335,90 @@
       <c r="C27" t="n">
         <v>26</v>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Kin | Sch</t>
+        </is>
+      </c>
       <c r="E27" t="n">
         <v>26</v>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Kin | Vor</t>
+        </is>
+      </c>
       <c r="G27" t="n">
         <v>26</v>
       </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Bad | Tec</t>
+        </is>
+      </c>
       <c r="I27" t="n">
         <v>26</v>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Gar</t>
+        </is>
+      </c>
       <c r="K27" t="n">
         <v>26</v>
       </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Kin</t>
+        </is>
+      </c>
       <c r="M27" t="n">
         <v>26</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Tec</t>
         </is>
       </c>
       <c r="O27" t="n">
         <v>26</v>
       </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Tec | WC</t>
+        </is>
+      </c>
       <c r="Q27" t="n">
         <v>26</v>
       </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Gar | Vor</t>
+        </is>
+      </c>
       <c r="S27" t="n">
         <v>26</v>
       </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Gar</t>
+        </is>
+      </c>
       <c r="U27" t="n">
         <v>26</v>
       </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Sch | Woh</t>
+        </is>
+      </c>
       <c r="W27" t="n">
         <v>26</v>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1678,37 +2428,82 @@
       <c r="C28" t="n">
         <v>27</v>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Tec</t>
+        </is>
+      </c>
       <c r="E28" t="n">
         <v>27</v>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Tec</t>
+        </is>
+      </c>
       <c r="G28" t="n">
         <v>27</v>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Gar | WC</t>
+        </is>
+      </c>
       <c r="I28" t="n">
         <v>27</v>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Vor | Woh</t>
+        </is>
+      </c>
       <c r="K28" t="n">
         <v>27</v>
       </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Tec | Vor</t>
+        </is>
+      </c>
       <c r="M28" t="n">
         <v>27</v>
       </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Bad | Gar</t>
+        </is>
+      </c>
       <c r="O28" t="n">
         <v>27</v>
       </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Sch | Gar</t>
+        </is>
+      </c>
       <c r="Q28" t="n">
         <v>27</v>
       </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="S28" t="n">
         <v>27</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>Kue</t>
+          <t>Bad | Woh</t>
         </is>
       </c>
       <c r="U28" t="n">
         <v>27</v>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
       </c>
       <c r="W28" t="n">
         <v>27</v>
@@ -1721,32 +2516,82 @@
       <c r="C29" t="n">
         <v>28</v>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Gar | Vor</t>
+        </is>
+      </c>
       <c r="E29" t="n">
         <v>28</v>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Gar</t>
+        </is>
+      </c>
       <c r="G29" t="n">
         <v>28</v>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Sch | Woh</t>
+        </is>
+      </c>
       <c r="I29" t="n">
         <v>28</v>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
+      </c>
       <c r="K29" t="n">
         <v>28</v>
       </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Gar</t>
+        </is>
+      </c>
       <c r="M29" t="n">
         <v>28</v>
       </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>WC | Woh</t>
+        </is>
+      </c>
       <c r="O29" t="n">
         <v>28</v>
       </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="Q29" t="n">
         <v>28</v>
       </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
+      </c>
       <c r="S29" t="n">
         <v>28</v>
       </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>Küc | WC</t>
+        </is>
+      </c>
       <c r="U29" t="n">
         <v>28</v>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
       </c>
       <c r="W29" t="n">
         <v>28</v>
@@ -1759,26 +2604,66 @@
       <c r="C30" t="n">
         <v>29</v>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="E30" t="n">
         <v>29</v>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Bad | Woh</t>
+        </is>
+      </c>
       <c r="G30" t="n">
         <v>29</v>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
+      </c>
       <c r="K30" t="n">
         <v>29</v>
       </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Woh</t>
+        </is>
+      </c>
       <c r="M30" t="n">
         <v>29</v>
       </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Sch | Küc</t>
+        </is>
+      </c>
       <c r="O30" t="n">
         <v>29</v>
       </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Küc | Vor</t>
+        </is>
+      </c>
       <c r="Q30" t="n">
         <v>29</v>
       </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
       <c r="S30" t="n">
         <v>29</v>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
       </c>
       <c r="U30" t="n">
         <v>29</v>
@@ -1794,15 +2679,35 @@
       <c r="C31" t="n">
         <v>30</v>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Küc</t>
+        </is>
+      </c>
       <c r="E31" t="n">
         <v>30</v>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Küc | WC</t>
+        </is>
+      </c>
       <c r="G31" t="n">
         <v>30</v>
       </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="K31" t="n">
         <v>30</v>
       </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Bad | Küc</t>
+        </is>
+      </c>
       <c r="M31" t="n">
         <v>30</v>
       </c>
@@ -1811,6 +2716,11 @@
       </c>
       <c r="Q31" t="n">
         <v>30</v>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
       </c>
       <c r="S31" t="n">
         <v>30</v>
@@ -1829,20 +2739,40 @@
       <c r="E32" t="n">
         <v>31</v>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Sch</t>
+        </is>
+      </c>
       <c r="G32" t="n">
         <v>31</v>
       </c>
       <c r="K32" t="n">
         <v>31</v>
       </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>WC</t>
+        </is>
+      </c>
       <c r="O32" t="n">
         <v>31</v>
       </c>
       <c r="S32" t="n">
         <v>31</v>
       </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>Vor</t>
+        </is>
+      </c>
       <c r="U32" t="n">
         <v>31</v>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>